<commit_message>
Updated paper with Pieter's feedback
</commit_message>
<xml_diff>
--- a/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
+++ b/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Functors" sheetId="1" r:id="rId1"/>
@@ -715,6 +715,7 @@
         <c:axId val="366035104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2970,7 +2971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -3547,8 +3548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Improved paper with better tables and coloured chart
</commit_message>
<xml_diff>
--- a/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
+++ b/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11616" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Functors" sheetId="1" r:id="rId1"/>
@@ -136,10 +136,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:prstDash val="sysDot"/>
               <a:round/>
@@ -151,17 +148,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="C00000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -261,7 +252,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:prstDash val="sysDot"/>
               <a:round/>
@@ -273,11 +264,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -377,9 +368,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
@@ -392,16 +382,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -463,7 +451,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
               <a:round/>
@@ -475,16 +465,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -546,9 +534,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="dash"/>
@@ -561,16 +548,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -632,7 +617,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="dash"/>
               <a:round/>
@@ -644,11 +631,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1823,9 +1814,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1847,7 +1838,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1858,7 +1849,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1869,7 +1860,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1880,7 +1871,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1891,7 +1882,7 @@
         <v>9.4700000000000003E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1902,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1913,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1924,7 +1915,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1935,7 +1926,7 @@
         <v>9.3999999999999994E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1946,7 +1937,7 @@
         <v>9.5100000000000002E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1957,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1968,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1979,7 +1970,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1990,7 +1981,7 @@
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2001,7 +1992,7 @@
         <v>9.5E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2012,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2023,7 +2014,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2034,7 +2025,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2045,7 +2036,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2056,7 +2047,7 @@
         <v>9.6000000000000002E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2067,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2078,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2089,7 +2080,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2100,7 +2091,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2111,7 +2102,7 @@
         <v>9.6500000000000004E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2122,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2133,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2144,7 +2135,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2155,7 +2146,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2166,7 +2157,7 @@
         <v>9.7099999999999997E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2177,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2188,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2199,7 +2190,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2210,7 +2201,7 @@
         <v>9.7E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2221,7 +2212,7 @@
         <v>9.7499999999999996E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2232,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2243,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2254,7 +2245,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2265,7 +2256,7 @@
         <v>9.7999999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2276,7 +2267,7 @@
         <v>9.8200000000000002E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2287,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2298,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2309,7 +2300,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2320,7 +2311,7 @@
         <v>9.8999999999999994E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2331,7 +2322,7 @@
         <v>9.9200000000000004E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2342,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2353,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2364,7 +2355,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2375,7 +2366,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2399,9 +2390,9 @@
       <selection activeCell="C49" activeCellId="9" sqref="C4:C6 C9:C11 C14:C16 C19:C21 C24:C26 C29:C31 C34:C36 C39:C41 C44:C46 C49:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2423,7 +2414,7 @@
         <v>1.1E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2434,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2445,7 +2436,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2456,7 +2447,7 @@
         <v>6.3E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2467,7 +2458,7 @@
         <v>7.2900000000000005E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2478,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2489,7 +2480,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2500,7 +2491,7 @@
         <v>1.2999999999999999E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2511,7 +2502,7 @@
         <v>1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2522,7 +2513,7 @@
         <v>1.7830000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2533,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2544,7 +2535,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2555,7 +2546,7 @@
         <v>2.6999999999999999E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2566,7 +2557,7 @@
         <v>3.0400000000000002E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2577,7 +2568,7 @@
         <v>3.3319999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2588,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2599,7 +2590,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2610,7 +2601,7 @@
         <v>4.5000000000000003E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2621,7 +2612,7 @@
         <v>5.0299999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2632,7 +2623,7 @@
         <v>5.4299999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2643,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2654,7 +2645,7 @@
         <v>6.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2665,7 +2656,7 @@
         <v>6.9999999999999994E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2676,7 +2667,7 @@
         <v>7.5199999999999996E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2687,7 +2678,7 @@
         <v>8.0269999999999994E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2698,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2709,7 +2700,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2720,7 +2711,7 @@
         <v>9.8999999999999994E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2731,7 +2722,7 @@
         <v>1.0510000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2742,7 +2733,7 @@
         <v>1.111E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2753,7 +2744,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2764,7 +2755,7 @@
         <v>1.2E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2775,7 +2766,7 @@
         <v>1.3300000000000001E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2786,7 +2777,7 @@
         <v>1.413E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2797,7 +2788,7 @@
         <v>1.4739E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2808,7 +2799,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2819,7 +2810,7 @@
         <v>1.7E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2830,7 +2821,7 @@
         <v>1.75E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2841,7 +2832,7 @@
         <v>1.8220000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2852,7 +2843,7 @@
         <v>1.8931E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2863,7 +2854,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2874,7 +2865,7 @@
         <v>2.0999999999999999E-5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2885,7 +2876,7 @@
         <v>2.2000000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2896,7 +2887,7 @@
         <v>2.294E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2907,7 +2898,7 @@
         <v>2.3666E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2918,7 +2909,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2929,7 +2920,7 @@
         <v>2.5999999999999998E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2940,7 +2931,7 @@
         <v>2.7E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2951,7 +2942,7 @@
         <v>2.8050000000000002E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2971,17 +2962,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2995,7 +2986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3017,7 +3008,7 @@
         <v>0.3124628755090797</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3035,7 +3026,7 @@
         <v>1.5238095238095239</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3053,7 +3044,7 @@
         <v>1.2990397805212619</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3071,7 +3062,7 @@
         <v>0.6923076923076924</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3089,7 +3080,7 @@
         <v>0.5911949685534591</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3107,7 +3098,7 @@
         <v>0.53337072349971959</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3125,7 +3116,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3143,7 +3134,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3161,7 +3152,7 @@
         <v>0.28511404561824732</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3179,7 +3170,7 @@
         <v>0.19999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3197,7 +3188,7 @@
         <v>0.19085487077534793</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -3215,7 +3206,7 @@
         <v>0.17679558011049726</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -3233,7 +3224,7 @@
         <v>0.12857142857142859</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -3251,7 +3242,7 @@
         <v>0.12765957446808512</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -3269,7 +3260,7 @@
         <v>0.12021925999750842</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -3287,7 +3278,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -3305,7 +3296,7 @@
         <v>9.1341579448144625E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -3323,7 +3314,7 @@
         <v>8.7398739873987399E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
@@ -3341,7 +3332,7 @@
         <v>6.7669172932330823E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7</v>
       </c>
@@ -3359,7 +3350,7 @@
         <v>6.8648266100495403E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
@@ -3377,7 +3368,7 @@
         <v>6.6151027885202524E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -3395,7 +3386,7 @@
         <v>5.1428571428571428E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -3413,7 +3404,7 @@
         <v>5.3787047200878152E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -3431,7 +3422,7 @@
         <v>5.1872589931857803E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -3449,7 +3440,7 @@
         <v>4.0909090909090909E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9</v>
       </c>
@@ -3467,7 +3458,7 @@
         <v>4.3156059285091537E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -3485,7 +3476,7 @@
         <v>4.1916673709118571E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -3503,7 +3494,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -3521,7 +3512,7 @@
         <v>3.5650623885918005E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10</v>
       </c>
@@ -3549,10 +3540,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed mistakes and expanded explanation on getVel
</commit_message>
<xml_diff>
--- a/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
+++ b/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11616" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Functors" sheetId="1" r:id="rId1"/>
@@ -769,7 +769,7 @@
         <c:axId val="359336512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000002E-2"/>
+          <c:max val="4.000000000000001E-3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1814,9 +1814,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>9.4700000000000003E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>9.3999999999999994E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>9.5100000000000002E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>9.5E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>9.6000000000000002E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>9.6500000000000004E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>9.7099999999999997E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>9.7E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>9.7499999999999996E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>9.7999999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>9.8200000000000002E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>9.8999999999999994E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>9.9200000000000004E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2390,9 +2390,9 @@
       <selection activeCell="C49" activeCellId="9" sqref="C4:C6 C9:C11 C14:C16 C19:C21 C24:C26 C29:C31 C34:C36 C39:C41 C44:C46 C49:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>1.1E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>6.3E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>7.2900000000000005E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>1.2999999999999999E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1.7830000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>2.6999999999999999E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>3.0400000000000002E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>3.3319999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>4.5000000000000003E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>5.0299999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>5.4299999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>6.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>6.9999999999999994E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>7.5199999999999996E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>8.0269999999999994E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>9.8999999999999994E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>1.0510000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>1.111E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>1.2E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>1.3300000000000001E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>1.413E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>1.4739E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>1.7E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>1.75E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>1.8220000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>1.8931E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>2.0999999999999999E-5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>2.2000000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>2.294E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>2.3666E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>1.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>2.5999999999999998E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>2.7E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>2.8050000000000002E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2966,13 +2966,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0.3124628755090797</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>1.5238095238095239</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>1.2990397805212619</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>0.6923076923076924</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>0.5911949685534591</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>0.53337072349971959</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>0.28511404561824732</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>0.19999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0.19085487077534793</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.17679558011049726</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>0.12857142857142859</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0.12765957446808512</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>0.12021925999750842</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>9.1341579448144625E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>8.7398739873987399E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>6.7669172932330823E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>6.8648266100495403E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>6.6151027885202524E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>5.1428571428571428E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>5.3787047200878152E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>5.1872589931857803E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>4.0909090909090909E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>4.3156059285091537E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>4.1916673709118571E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>3.5650623885918005E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -3540,10 +3540,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed final version of the paper
</commit_message>
<xml_diff>
--- a/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
+++ b/20. Metacasanova (WAPL)/Evaluation/Evaluation.xlsx
@@ -86,6 +86,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4C0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -136,7 +141,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="4C0000"/>
               </a:solidFill>
               <a:prstDash val="sysDot"/>
               <a:round/>
@@ -148,11 +153,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="4C0000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="C00000"/>
+                  <a:srgbClr val="4C0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -3539,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>